<commit_message>
Use markdown to fill junior progress report
</commit_message>
<xml_diff>
--- a/platform/src/main/resources/jxls/admin_junior_registry_template.xlsx
+++ b/platform/src/main/resources/jxls/admin_junior_registry_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stm\hreasy\src\hreasy\platform\src\main\resources\jxls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\stm\hreasy\src\hreasy\platform\src\main\resources\jxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6AB887-ECD1-4090-B03D-DBD0942B1329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F704D2-F0D6-4999-8010-4F9633B834CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Реестр молодых специалистов" sheetId="1" r:id="rId1"/>
@@ -525,9 +525,6 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -551,9 +548,7 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -566,9 +561,14 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,7 +663,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -803,7 +803,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -943,7 +943,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1083,7 +1083,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1187,7 +1187,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1292,7 +1292,7 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1954,8 +1954,8 @@
   <dimension ref="A1:AC10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G22" sqref="G22"/>
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,11 +1991,11 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -2024,13 +2024,13 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="27">
+      <c r="F2" s="21">
         <v>1</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="28"/>
+      <c r="H2" s="26"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -2059,13 +2059,13 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="27">
+      <c r="F3" s="21">
         <v>2</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="28"/>
+      <c r="H3" s="26"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -2094,13 +2094,13 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="27">
+      <c r="F4" s="21">
         <v>3</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="H4" s="28"/>
+      <c r="H4" s="26"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -2129,13 +2129,13 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="27">
+      <c r="F5" s="21">
         <v>4</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="28"/>
+      <c r="H5" s="26"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2193,49 +2193,49 @@
       <c r="AC6" s="2"/>
     </row>
     <row r="7" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="23" t="s">
+      <c r="H7" s="24"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23" t="s">
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23" t="s">
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23" t="s">
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23" t="s">
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="23"/>
+      <c r="AA7" s="22"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
     </row>
     <row r="8" spans="1:29" s="8" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -2326,128 +2326,133 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:29" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="12" t="s">
         <v>19</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="M9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="N9" s="14" t="s">
+      <c r="N9" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="O9" s="13" t="s">
+      <c r="O9" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="P9" s="10" t="s">
+      <c r="P9" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="Q9" s="14" t="s">
+      <c r="Q9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="R9" s="14" t="s">
+      <c r="R9" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="S9" s="13" t="s">
+      <c r="S9" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="T9" s="10" t="s">
+      <c r="T9" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="U9" s="14" t="s">
+      <c r="U9" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="V9" s="14" t="s">
+      <c r="V9" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="W9" s="13" t="s">
+      <c r="W9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="X9" s="10" t="s">
+      <c r="X9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="Y9" s="14" t="s">
+      <c r="Y9" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="Z9" s="14" t="s">
+      <c r="Z9" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="AA9" s="13" t="s">
+      <c r="AA9" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="AB9" s="10" t="s">
+      <c r="AB9" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="AC9" s="14" t="s">
+      <c r="AC9" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="18"/>
-      <c r="AA10" s="19"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="18"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="G2:H2"/>
     <mergeCell ref="R7:U7"/>
     <mergeCell ref="V7:Y7"/>
     <mergeCell ref="Z7:AC7"/>
@@ -2455,11 +2460,6 @@
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="J7:M7"/>
     <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>